<commit_message>
Sesión 2 - Pizarrón
</commit_message>
<xml_diff>
--- a/Proyecto1.xlsx
+++ b/Proyecto1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Documents/Cursos 2025/INEGI-GIT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE83C7B5-AFDD-2D46-A6A6-8967037E7B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C3136D-823C-F34E-A7EB-D404011D20EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{8AD61B31-4F1C-5C40-AB95-A227DDFF3857}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{8AD61B31-4F1C-5C40-AB95-A227DDFF3857}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="101">
   <si>
     <t>Proyecto A</t>
   </si>
@@ -337,13 +338,16 @@
   </si>
   <si>
     <t>r63</t>
+  </si>
+  <si>
+    <t>c20c68c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -354,6 +358,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -409,16 +420,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -426,6 +444,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,21 +792,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9F4A3F-D9DF-2343-A21E-6ECE7CCEF563}">
   <dimension ref="A3:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="237" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A2" zoomScale="237" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -784,18 +814,18 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
@@ -807,10 +837,10 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -835,33 +865,33 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="11" t="s">
         <v>14</v>
       </c>
       <c r="G8" t="s">
@@ -958,7 +988,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
@@ -966,7 +996,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
@@ -997,7 +1027,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B19" t="s">
@@ -1005,7 +1035,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1021,17 +1051,174 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC58018A-37E0-4341-902B-0BA34F45F3E8}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView zoomScale="257" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97151905-8C2F-C54C-B2DD-98282B5D2D53}">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView zoomScale="322" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="322" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="4" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
   </cols>
@@ -1043,7 +1230,7 @@
       <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="14" t="s">
         <v>93</v>
       </c>
       <c r="E2" t="s">
@@ -1060,7 +1247,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
@@ -1069,10 +1256,10 @@
       <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="16">
         <v>123</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F3" t="s">
@@ -1083,17 +1270,17 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="16">
         <v>123</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F4" t="s">
@@ -1104,17 +1291,17 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="16">
         <v>123</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F5" t="s">
@@ -1125,17 +1312,17 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="16">
         <v>123</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F6" t="s">
@@ -1146,17 +1333,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="D7">
-        <v>123</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F7" t="s">
@@ -1170,17 +1357,17 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>72</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="16">
         <v>123</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F8" t="s">
@@ -1194,17 +1381,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>75</v>
       </c>
       <c r="C9" t="s">
         <v>75</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="16">
         <v>123</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F9" t="s">
@@ -1213,22 +1400,22 @@
       <c r="G9" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>86</v>
       </c>
       <c r="C10" t="s">
         <v>86</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="16">
         <v>123</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F10" t="s">
@@ -1242,17 +1429,17 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>87</v>
       </c>
       <c r="C11" t="s">
         <v>87</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="16">
         <v>123</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F11" t="s">
@@ -1266,17 +1453,17 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
       <c r="C12" t="s">
         <v>77</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="16">
         <v>123</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F12" t="s">
@@ -1290,17 +1477,17 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>75</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="16">
         <v>123</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F13" t="s">
@@ -1309,22 +1496,22 @@
       <c r="G13" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>89</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="16">
         <v>123</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F14" t="s">
@@ -1338,17 +1525,17 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>83</v>
       </c>
       <c r="C15" t="s">
         <v>83</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="16">
         <v>123</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>84</v>
       </c>
       <c r="F15" t="s">
@@ -1362,17 +1549,17 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>75</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="16">
         <v>123</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>84</v>
       </c>
       <c r="F16" t="s">
@@ -1381,12 +1568,12 @@
       <c r="G16" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="12" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
@@ -1395,10 +1582,10 @@
       <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>95</v>
       </c>
       <c r="F17" t="s">
@@ -1412,17 +1599,17 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>57</v>
       </c>
       <c r="C18" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>96</v>
       </c>
       <c r="F18" t="s">
@@ -1436,17 +1623,17 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>97</v>
       </c>
       <c r="F19" t="s">
@@ -1460,17 +1647,17 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2"/>
       <c r="B20" t="s">
         <v>59</v>
       </c>
       <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F20" t="s">
@@ -1484,17 +1671,17 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
       <c r="B21" t="s">
         <v>60</v>
       </c>
       <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F21" t="s">
@@ -1502,31 +1689,31 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>